<commit_message>
fixed some stuff in magnitude
</commit_message>
<xml_diff>
--- a/lab_first_year/second_semester/magnitude/עותק של נתונים(547).xlsx
+++ b/lab_first_year/second_semester/magnitude/עותק של נתונים(547).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\PycharmProjects\physics_python_tools\lab_first_year\second_semester\magnitude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F65A90FE-5D3C-4D45-A459-F0D8AEE76C85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A25002F-8E70-4EF2-B89F-570F0BA25C94}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16410" windowHeight="7575" xr2:uid="{3978E05C-874F-41E8-ACF5-E549344A537F}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>theta</t>
   </si>
@@ -109,13 +109,29 @@
   <si>
     <t>dfield[mT]</t>
   </si>
+  <si>
+    <t>\mu_0</t>
+  </si>
+  <si>
+    <t>עמודה1</t>
+  </si>
+  <si>
+    <t>עמודה2</t>
+  </si>
+  <si>
+    <t>rfield</t>
+  </si>
+  <si>
+    <t>rdfield</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -152,22 +168,48 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="15">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2250,16 +2292,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>338138</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>28294</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>461402</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>151559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>109537</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>56869</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>232801</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>839</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2286,16 +2328,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1237450</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>46745</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>430626</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>125186</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>359389</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>138953</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>191302</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2328,7 +2370,7 @@
   <autoFilter ref="A35:F72" xr:uid="{0DC03297-4F76-4D23-A1EC-1D338CAAC6AB}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{779AF918-A70E-427E-B698-02E5FA7456E0}" name="theta"/>
-    <tableColumn id="2" xr3:uid="{5167D406-BF7B-4237-A9C5-2DD031AE996A}" name="theta(rad)" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{5167D406-BF7B-4237-A9C5-2DD031AE996A}" name="theta(rad)" dataDxfId="14">
       <calculatedColumnFormula>טבלה1[[#This Row],[theta]]*PI()/180</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{2C0C528B-3D7E-4D66-B2C4-0E0DF84686E4}" name="dtheta">
@@ -2336,7 +2378,7 @@
     </tableColumn>
     <tableColumn id="4" xr3:uid="{DAD78F71-4561-4D8D-A68F-ED1C5EFF0003}" name="field"/>
     <tableColumn id="5" xr3:uid="{B19CCBA4-9035-4B80-849D-6C44867247B4}" name="dfield"/>
-    <tableColumn id="6" xr3:uid="{ACD1EE3B-40CB-446F-B457-5EABDEB6845D}" name="d/field %" dataDxfId="5">
+    <tableColumn id="6" xr3:uid="{ACD1EE3B-40CB-446F-B457-5EABDEB6845D}" name="d/field %" dataDxfId="13">
       <calculatedColumnFormula>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2353,12 +2395,12 @@
       <calculatedColumnFormula>B$4/SQRT(12)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{FB739B05-AA99-4F0F-AC35-F2727CE11DA0}" name="field"/>
-    <tableColumn id="4" xr3:uid="{B5037E0A-A106-4A71-A9CB-F069D01943C8}" name="d_field" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{7F8EF07D-35BC-4DB4-BA3B-773C494F9E80}" name="d_field_stat" dataDxfId="3">
+    <tableColumn id="4" xr3:uid="{B5037E0A-A106-4A71-A9CB-F069D01943C8}" name="d_field" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{7F8EF07D-35BC-4DB4-BA3B-773C494F9E80}" name="d_field_stat" dataDxfId="11">
       <calculatedColumnFormula>טבלה2[[#This Row],[d_field]]/COUNT(טבלה2[d_field])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{6B51AC54-8FB2-4B9C-A337-4F8DC4D8BBB7}" name="d_inst"/>
-    <tableColumn id="7" xr3:uid="{8C8E61C3-32E4-4C03-A53E-F76A482DA22D}" name="D_field_final[mT]" dataDxfId="2">
+    <tableColumn id="7" xr3:uid="{8C8E61C3-32E4-4C03-A53E-F76A482DA22D}" name="D_field_final[mT]" dataDxfId="10">
       <calculatedColumnFormula>SQRT(טבלה2[[#This Row],[d_inst]]^2+טבלה2[[#This Row],[d_field_stat]]^2)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2367,20 +2409,50 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53DF2BAF-71A0-4178-B157-1386398B5DA9}" name="טבלה3" displayName="טבלה3" ref="I5:L26" totalsRowShown="0">
-  <autoFilter ref="I5:L26" xr:uid="{4FF7C998-436B-4A1A-919F-0317CDF5E2C5}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53DF2BAF-71A0-4178-B157-1386398B5DA9}" name="טבלה3" displayName="טבלה3" ref="I5:N26" totalsRowShown="0">
+  <autoFilter ref="I5:N26" xr:uid="{4FF7C998-436B-4A1A-919F-0317CDF5E2C5}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{AB4EF37C-7480-4BA6-BD27-5639B598CF43}" name="r[m]">
       <calculatedColumnFormula>טבלה2[[#This Row],[r]]/100</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{CD187CD8-1E82-43AE-9D16-14837BD9D80B}" name="dr[m]">
-      <calculatedColumnFormula>טבלה2[[#This Row],[dr]]/100</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{CD187CD8-1E82-43AE-9D16-14837BD9D80B}" name="dr[m]" dataDxfId="9">
+      <calculatedColumnFormula>טבלה2[[#This Row],[dr]]/10</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BB803144-08EE-48CD-BE20-91F9358C99CE}" name="field[mT]" dataDxfId="1">
-      <calculatedColumnFormula>טבלה2[[#This Row],[field]]-B$2</calculatedColumnFormula>
+    <tableColumn id="3" xr3:uid="{BB803144-08EE-48CD-BE20-91F9358C99CE}" name="field[mT]" dataDxfId="2">
+      <calculatedColumnFormula>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{757FE207-AE66-47D1-BD8A-2FCD514CB17D}" name="dfield[mT]" dataDxfId="0">
-      <calculatedColumnFormula>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</calculatedColumnFormula>
+    <tableColumn id="4" xr3:uid="{757FE207-AE66-47D1-BD8A-2FCD514CB17D}" name="dfield[mT]" dataDxfId="3">
+      <calculatedColumnFormula>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{7D175972-46C2-4F8A-875B-F977AD59AB92}" name="עמודה1" dataDxfId="8">
+      <calculatedColumnFormula>ABS((טבלה2[[#This Row],[field]]-B$2))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{C21BB12E-2DE9-4A15-9ED0-83CFC10A82A8}" name="עמודה2" dataDxfId="7">
+      <calculatedColumnFormula>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{28460B4E-1C5E-47C0-81B1-3FD64617BCAB}" name="טבלה4" displayName="טבלה4" ref="H35:L72" totalsRowShown="0">
+  <autoFilter ref="H35:L72" xr:uid="{472B2439-8FB4-4D68-BF2C-BB9F42296F15}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{A7CE6F21-3D6B-45D2-908C-B01D61845575}" name="theta" dataDxfId="5">
+      <calculatedColumnFormula>טבלה1[[#This Row],[theta(rad)]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{75B04DF4-57EC-4869-A85F-8755D7CC3E5E}" name="dtheta" dataDxfId="4">
+      <calculatedColumnFormula>טבלה1[[#This Row],[dtheta]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{97128DD4-6A07-424A-93F2-E73080F3C453}" name="rfield" dataDxfId="1">
+      <calculatedColumnFormula>(טבלה1[[#This Row],[field]]-B$2)/B$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{BB0751EB-1985-4C71-91E2-1CC4C179CC7F}" name="rdfield" dataDxfId="0">
+      <calculatedColumnFormula>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{F15FAA57-0C17-49D4-AAA3-674F9A125419}" name="עמודה1" dataDxfId="6">
+      <calculatedColumnFormula>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2684,14 +2756,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACB3525-4999-4FD4-93CD-2A2019125F89}">
-  <dimension ref="A1:L72"/>
+  <dimension ref="A1:N72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61:L61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.625" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
     <col min="7" max="7" width="11.375" customWidth="1"/>
@@ -2700,7 +2773,7 @@
     <col min="12" max="12" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>5</v>
       </c>
@@ -2708,7 +2781,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2721,8 +2794,21 @@
       <c r="D2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f>SQRT(0.001^2 + C2 ^2)</f>
+        <v>1.0645304129051456E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3">
+        <f>4*PI()*10^-7</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2736,7 +2822,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2770,8 +2856,14 @@
       <c r="L5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>25</v>
       </c>
@@ -2800,20 +2892,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.25</v>
       </c>
-      <c r="J6">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J6" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K6">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-0.20900000000000002</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>166316.91553103065</v>
       </c>
       <c r="L6">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646230955605402E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.327611551721</v>
+      </c>
+      <c r="M6">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>0.20900000000000002</v>
+      </c>
+      <c r="N6" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>5561.376131826416</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>26</v>
       </c>
@@ -2842,20 +2942,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.26</v>
       </c>
-      <c r="J7">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J7" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K7">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-0.159</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>126528.17975805679</v>
       </c>
       <c r="L7">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0645969769617087E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3124621675709</v>
+      </c>
+      <c r="M7">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>0.159</v>
+      </c>
+      <c r="N7" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>7310.1412714941562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>27</v>
       </c>
@@ -2884,20 +2992,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.27</v>
       </c>
-      <c r="J8">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J8" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K8">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-0.126</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>100267.61414789407</v>
       </c>
       <c r="L8">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0645917584900316E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3094353556337</v>
+      </c>
+      <c r="M8">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>0.126</v>
+      </c>
+      <c r="N8" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>9224.6780583780455</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>28</v>
       </c>
@@ -2926,20 +3042,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="J9">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J9" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K9">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-0.10100000000000001</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>80373.246261407156</v>
       </c>
       <c r="L9">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646334214157777E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3336008317633</v>
+      </c>
+      <c r="M9">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="N9" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>11508.253473581814</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>29</v>
       </c>
@@ -2968,20 +3092,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.28999999999999998</v>
       </c>
-      <c r="J10">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J10" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K10">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-8.199999999999999E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>65253.526667677077</v>
       </c>
       <c r="L10">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646199805319481E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3258047548075</v>
+      </c>
+      <c r="M10">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>8.199999999999999E-2</v>
+      </c>
+      <c r="N10" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>14174.704936034239</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>30</v>
       </c>
@@ -3010,20 +3142,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.3</v>
       </c>
-      <c r="J11">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J11" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K11">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-6.8000000000000005E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>54112.680651244416</v>
       </c>
       <c r="L11">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0645778293053663E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3013562000303</v>
+      </c>
+      <c r="M11">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="N11" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>17092.66700294162</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>31</v>
       </c>
@@ -3052,20 +3192,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.31</v>
       </c>
-      <c r="J12">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J12" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K12">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-5.6000000000000001E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>44563.384065730694</v>
       </c>
       <c r="L12">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646676698226223E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3534660446285</v>
+      </c>
+      <c r="M12">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="N12" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>20756.311893654078</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>32</v>
       </c>
@@ -3094,20 +3242,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.32</v>
       </c>
-      <c r="J13">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J13" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K13">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-4.8100000000000004E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>38276.763813600832</v>
       </c>
       <c r="L13">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0645969769617087E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3124621675709</v>
+      </c>
+      <c r="M13">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>4.8100000000000004E-2</v>
+      </c>
+      <c r="N13" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>24164.500252964048</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>33</v>
       </c>
@@ -3136,20 +3292,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.33</v>
       </c>
-      <c r="J14">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J14" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K14">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-4.2000000000000003E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>33422.538049298026</v>
       </c>
       <c r="L14">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646103702119437E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3202305369898</v>
+      </c>
+      <c r="M14">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="N14" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>27674.291203261659</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>34</v>
       </c>
@@ -3178,20 +3342,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.34</v>
       </c>
-      <c r="J15">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J15" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K15">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-3.5999999999999997E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>28647.889756541157</v>
       </c>
       <c r="L15">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.064618749427537E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3250906831845</v>
+      </c>
+      <c r="M15">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="N15" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>32286.808074532906</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>35</v>
       </c>
@@ -3220,20 +3392,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.35</v>
       </c>
-      <c r="J16">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J16" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K16">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-3.1800000000000002E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>25305.635951611359</v>
       </c>
       <c r="L16">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646513636290037E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3440078736808</v>
+      </c>
+      <c r="M16">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>3.1800000000000002E-2</v>
+      </c>
+      <c r="N16" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>36551.698360807568</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>36</v>
       </c>
@@ -3262,20 +3442,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.36</v>
       </c>
-      <c r="J17">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J17" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K17">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-2.8000000000000001E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>22281.692032865347</v>
       </c>
       <c r="L17">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0645862641572076E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.306248546548</v>
+      </c>
+      <c r="M17">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="N17" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>41510.937448090997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>37</v>
       </c>
@@ -3304,20 +3492,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.37</v>
       </c>
-      <c r="J18">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J18" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K18">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-2.5000000000000001E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>19894.367886486918</v>
       </c>
       <c r="L18">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646230955605402E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.327611551721</v>
+      </c>
+      <c r="M18">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="N18" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>46493.104462068841</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>38</v>
       </c>
@@ -3346,20 +3542,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.38</v>
       </c>
-      <c r="J19">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J19" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K19">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-2.3E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>18302.818455567962</v>
       </c>
       <c r="L19">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646387887762183E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3367140591988</v>
+      </c>
+      <c r="M19">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>2.3E-2</v>
+      </c>
+      <c r="N19" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>50536.378872139081</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>39</v>
       </c>
@@ -3388,20 +3592,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.39</v>
       </c>
-      <c r="J20">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J20" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K20">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-2.1000000000000001E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>16711.269024649013</v>
       </c>
       <c r="L20">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646151072244898E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3229781157797</v>
+      </c>
+      <c r="M20">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="N20" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>55348.713243608552</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>40</v>
       </c>
@@ -3430,20 +3642,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.4</v>
       </c>
-      <c r="J21">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J21" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K21">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-1.9E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>15119.719593730057</v>
       </c>
       <c r="L21">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0645743019838702E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.2993103035624</v>
+      </c>
+      <c r="M21">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>1.9E-2</v>
+      </c>
+      <c r="N21" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>61173.647910713808</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>41</v>
       </c>
@@ -3472,20 +3692,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.41</v>
       </c>
-      <c r="J22">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J22" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K22">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-1.7000000000000001E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>13528.170162811104</v>
       </c>
       <c r="L22">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646109548848213E-3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3205696607124</v>
+      </c>
+      <c r="M22">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="N22" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>68371.798215336021</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>42</v>
       </c>
@@ -3514,20 +3742,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.42</v>
       </c>
-      <c r="J23">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J23" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K23">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-1.6E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>12732.395447351628</v>
       </c>
       <c r="L23">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646163127737784E-3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3236773636618</v>
+      </c>
+      <c r="M23">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>1.6E-2</v>
+      </c>
+      <c r="N23" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>72645.229835228864</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>43</v>
       </c>
@@ -3556,20 +3792,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.43</v>
       </c>
-      <c r="J24">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J24" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K24">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-1.4999999999999999E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>11936.62073189215</v>
       </c>
       <c r="L24">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.064581492936093E-3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3034811611485</v>
+      </c>
+      <c r="M24">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="N24" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>77486.898744076563</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>44</v>
       </c>
@@ -3598,20 +3842,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.44</v>
       </c>
-      <c r="J25">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J25" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K25">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-1.3999999999999999E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>11140.846016432672</v>
       </c>
       <c r="L25">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0645927851464807E-3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3100308351763</v>
+      </c>
+      <c r="M25">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="N25" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>83022.145059655464</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>45</v>
       </c>
@@ -3640,20 +3892,28 @@
         <f>טבלה2[[#This Row],[r]]/100</f>
         <v>0.45</v>
       </c>
-      <c r="J26">
-        <f>טבלה2[[#This Row],[dr]]/100</f>
-        <v>2.8867513459481289E-5</v>
+      <c r="J26" s="5">
+        <f>טבלה2[[#This Row],[dr]]/10</f>
+        <v>2.886751345948129E-4</v>
       </c>
       <c r="K26">
-        <f>טבלה2[[#This Row],[field]]-B$2</f>
-        <v>-1.3000000000000001E-2</v>
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2)/B$3)</f>
+        <v>10345.071300973197</v>
       </c>
       <c r="L26">
-        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +C$2^2)</f>
-        <v>1.0646069068971666E-3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <f>SQRT(טבלה2[[#This Row],[D_field_final'[mT']]]^2 +E$2^2)/B$3</f>
+        <v>1162.3182217365161</v>
+      </c>
+      <c r="M26">
+        <f>ABS((טבלה2[[#This Row],[field]]-B$2))</f>
+        <v>1.3000000000000001E-2</v>
+      </c>
+      <c r="N26" s="6">
+        <f>טבלה3[[#This Row],[dfield'[mT']]]/טבלה3[[#This Row],[עמודה1]]</f>
+        <v>89409.093979732002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -3661,7 +3921,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -3669,7 +3929,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -3688,8 +3948,23 @@
       <c r="F35" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>0</v>
+      </c>
+      <c r="I35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J35" t="s">
+        <v>29</v>
+      </c>
+      <c r="K35" t="s">
+        <v>30</v>
+      </c>
+      <c r="L35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0</v>
       </c>
@@ -3711,8 +3986,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>1.811965811965812</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H36">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>0</v>
+      </c>
+      <c r="I36">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J36">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-30942.108261210833</v>
+      </c>
+      <c r="K36">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>863.76167723911772</v>
+      </c>
+      <c r="L36" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-2.791541125599167E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>10</v>
       </c>
@@ -3734,8 +4029,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>0.34581772784019976</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H37">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>0.17453292519943295</v>
+      </c>
+      <c r="I37">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J37">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-30397.798355836549</v>
+      </c>
+      <c r="K37">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>875.33554792141399</v>
+      </c>
+      <c r="L37" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-2.8796017977181714E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>20</v>
       </c>
@@ -3757,8 +4072,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>8.9285714285714288E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H38">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>0.3490658503988659</v>
+      </c>
+      <c r="I38">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J38">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-28807.044699633057</v>
+      </c>
+      <c r="K38">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>870.17337464558716</v>
+      </c>
+      <c r="L38" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-3.0206964432442158E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>30</v>
       </c>
@@ -3780,8 +4115,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>4.0819672131147539E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H39">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>0.52359877559829882</v>
+      </c>
+      <c r="I39">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J39">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-26180.988138616784</v>
+      </c>
+      <c r="K39">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>869.9917853063929</v>
+      </c>
+      <c r="L39" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-3.3229906400024711E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>40</v>
       </c>
@@ -3803,8 +4158,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>2.4636363636363637E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H40">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>0.69813170079773179</v>
+      </c>
+      <c r="I40">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J40">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-22281.692032865347</v>
+      </c>
+      <c r="K40">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>874.1453947319244</v>
+      </c>
+      <c r="L40" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-3.9231553575130911E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>50</v>
       </c>
@@ -3826,8 +4201,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>1.7124999999999998E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H41">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>0.87266462599716477</v>
+      </c>
+      <c r="I41">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J41">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-18302.818455567962</v>
+      </c>
+      <c r="K41">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>874.73741601487313</v>
+      </c>
+      <c r="L41" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-4.7792498086477293E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>60</v>
       </c>
@@ -3849,8 +4244,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>8.7619047619047607E-3</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H42">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>1.0471975511965976</v>
+      </c>
+      <c r="I42">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J42">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-14323.944878270579</v>
+      </c>
+      <c r="K42">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>859.687546170421</v>
+      </c>
+      <c r="L42" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-6.0017512876258471E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>70</v>
       </c>
@@ -3872,8 +4287,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>9.703703703703704E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H43">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>1.2217304763960306</v>
+      </c>
+      <c r="I43">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J43">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-9549.2965855137209</v>
+      </c>
+      <c r="K43">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>872.40611838406733</v>
+      </c>
+      <c r="L43" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-9.1358155082072443E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>80</v>
       </c>
@@ -3895,8 +4330,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>9.8823529411764689E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H44">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>1.3962634015954636</v>
+      </c>
+      <c r="I44">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J44">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-3978.8735772973814</v>
+      </c>
+      <c r="K44">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>888.32164319002982</v>
+      </c>
+      <c r="L44" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-0.22325957986164902</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>90</v>
       </c>
@@ -3918,8 +4373,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>6.5121951219512192E-3</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H45">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>1.5707963267948966</v>
+      </c>
+      <c r="I45">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J45">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>1591.5494309189548</v>
+      </c>
+      <c r="K45">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>873.36555989519206</v>
+      </c>
+      <c r="L45" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>0.54875176537301384</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>100</v>
       </c>
@@ -3941,8 +4416,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>7.3043478260869559E-3</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H46">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>1.7453292519943295</v>
+      </c>
+      <c r="I46">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J46">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>5570.4230082163358</v>
+      </c>
+      <c r="K46">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>888.32164319002982</v>
+      </c>
+      <c r="L46" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>0.15947112847260639</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>110</v>
       </c>
@@ -3964,8 +4459,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>4.5961538461538462E-3</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H47">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>1.9198621771937625</v>
+      </c>
+      <c r="I47">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J47">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>10345.071300973195</v>
+      </c>
+      <c r="K47">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>868.21391972227309</v>
+      </c>
+      <c r="L47" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>8.3925368367504374E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>120</v>
       </c>
@@ -3987,8 +4502,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>5.5689655172413786E-3</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H48">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>2.0943951023931953</v>
+      </c>
+      <c r="I48">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J48">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>15119.719593730058</v>
+      </c>
+      <c r="K48">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>885.26280032156853</v>
+      </c>
+      <c r="L48" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>5.855021284182247E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>130</v>
       </c>
@@ -4010,8 +4545,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>2.6718750000000002E-3</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H49">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>2.2689280275926285</v>
+      </c>
+      <c r="I49">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J49">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>19894.367886486918</v>
+      </c>
+      <c r="K49">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>857.98612701478817</v>
+      </c>
+      <c r="L49" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>4.3127086616185882E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>140</v>
       </c>
@@ -4033,8 +4588,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.1029411764705883E-3</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H50">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>2.4434609527920612</v>
+      </c>
+      <c r="I50">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J50">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>23077.466748324827</v>
+      </c>
+      <c r="K50">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>863.60660441411596</v>
+      </c>
+      <c r="L50" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>3.7422071227848457E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>150</v>
       </c>
@@ -4056,8 +4631,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.5416666666666674E-3</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H51">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>2.6179938779914944</v>
+      </c>
+      <c r="I51">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J51">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>26260.565610162725</v>
+      </c>
+      <c r="K51">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>871.09165813446123</v>
+      </c>
+      <c r="L51" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>3.317109277331607E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>160</v>
       </c>
@@ -4079,8 +4674,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.9473684210526317E-3</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H52">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>2.7925268031909272</v>
+      </c>
+      <c r="I52">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J52">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>29443.664472000637</v>
+      </c>
+      <c r="K52">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>880.12287800091644</v>
+      </c>
+      <c r="L52" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>2.9891757489556595E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>170</v>
       </c>
@@ -4102,8 +4717,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.6753246753246753E-3</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H53">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>2.9670597283903604</v>
+      </c>
+      <c r="I53">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J53">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>30239.439187460113</v>
+      </c>
+      <c r="K53">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>876.55009344096868</v>
+      </c>
+      <c r="L53" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>2.8986982463764147E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>180</v>
       </c>
@@ -4125,8 +4760,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.1265822784810123E-3</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H54">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>3.1415926535897931</v>
+      </c>
+      <c r="I54">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J54">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>31830.98861837907</v>
+      </c>
+      <c r="K54">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>869.63067744992884</v>
+      </c>
+      <c r="L54" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>2.7320253476130114E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>190</v>
       </c>
@@ -4148,8 +4803,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>5.3974358974358972E-3</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H55">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>3.3161255787892263</v>
+      </c>
+      <c r="I55">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J55">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>31035.21390291959</v>
+      </c>
+      <c r="K55">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>910.96777605961381</v>
+      </c>
+      <c r="L55" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>2.9352714594111946E-2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>200</v>
       </c>
@@ -4171,8 +4846,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>4.8000000000000004E-3</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H56">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>3.4906585039886591</v>
+      </c>
+      <c r="I56">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J56">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>28647.889756541157</v>
+      </c>
+      <c r="K56">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>894.25570914145953</v>
+      </c>
+      <c r="L56" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>3.1215412958550449E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>210</v>
       </c>
@@ -4194,8 +4889,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.3972602739726029E-3</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H57">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>3.6651914291880923</v>
+      </c>
+      <c r="I57">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J57">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>27056.340325622205</v>
+      </c>
+      <c r="K57">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>869.81088609761366</v>
+      </c>
+      <c r="L57" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>3.2148135173843434E-2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>220</v>
       </c>
@@ -4217,8 +4932,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.7101449275362313E-3</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H58">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>3.839724354387525</v>
+      </c>
+      <c r="I58">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J58">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>23873.241463784307</v>
+      </c>
+      <c r="K58">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>871.27737914036459</v>
+      </c>
+      <c r="L58" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>3.649598151395117E-2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>230</v>
       </c>
@@ -4240,8 +4975,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>4.5555555555555549E-3</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H59">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>4.0142572795869578</v>
+      </c>
+      <c r="I59">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J59">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>19098.593171027442</v>
+      </c>
+      <c r="K59">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>877.373291808153</v>
+      </c>
+      <c r="L59" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>4.5939158133339784E-2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>240</v>
       </c>
@@ -4263,8 +5018,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>4.3103448275862068E-3</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H60">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>4.1887902047863905</v>
+      </c>
+      <c r="I60">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J60">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>15119.719593730058</v>
+      </c>
+      <c r="K60">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>870.17337464558716</v>
+      </c>
+      <c r="L60" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>5.7552216444968739E-2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>250</v>
       </c>
@@ -4286,8 +5061,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>3.8823529411764705E-3</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H61">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>4.3633231299858233</v>
+      </c>
+      <c r="I61">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J61">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>9549.2965855137172</v>
+      </c>
+      <c r="K61">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>861.65499917528768</v>
+      </c>
+      <c r="L61" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>9.0232300511266794E-2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>260</v>
       </c>
@@ -4309,8 +5104,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>5.4888888888888886E-3</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H62">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>4.5378560551852569</v>
+      </c>
+      <c r="I62">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J62">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>4774.6482927568586</v>
+      </c>
+      <c r="K62">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>869.63067744992884</v>
+      </c>
+      <c r="L62" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>0.18213502317420083</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>270</v>
       </c>
@@ -4332,8 +5147,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>7.5384615384615382E-3</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H63">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>4.7123889803846897</v>
+      </c>
+      <c r="I63">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J63">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>878.83977550801774</v>
+      </c>
+      <c r="L63" s="6" t="e">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>280</v>
       </c>
@@ -4355,8 +5190,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>9.4062499999999997E-3</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H64">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>4.8869219055841224</v>
+      </c>
+      <c r="I64">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J64">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-5570.4230082163358</v>
+      </c>
+      <c r="K64">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>880.33906426823569</v>
+      </c>
+      <c r="L64" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-0.15803809925561157</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>290</v>
       </c>
@@ -4378,8 +5233,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>1.392E-2</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H65">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>5.0614548307835552</v>
+      </c>
+      <c r="I65">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J65">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-11140.846016432672</v>
+      </c>
+      <c r="K65">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>891.24245774126291</v>
+      </c>
+      <c r="L65" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-7.9997735937350392E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>300</v>
       </c>
@@ -4401,8 +5276,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>1.5842105263157893E-2</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H66">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>5.2359877559829888</v>
+      </c>
+      <c r="I66">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J66">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-15915.494309189535</v>
+      </c>
+      <c r="K66">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>880.33906426823569</v>
+      </c>
+      <c r="L66" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-5.5313334739464037E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>310</v>
       </c>
@@ -4424,8 +5319,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>1.5642857142857142E-2</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H67">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>5.4105206811824216</v>
+      </c>
+      <c r="I67">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J67">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-19894.367886486918</v>
+      </c>
+      <c r="K67">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>864.86691036019511</v>
+      </c>
+      <c r="L67" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-4.3472952510727858E-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>320</v>
       </c>
@@ -4447,8 +5362,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>2.9111111111111115E-2</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H68">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>5.5850536063818543</v>
+      </c>
+      <c r="I68">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J68">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-23873.241463784299</v>
+      </c>
+      <c r="K68">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>872.40611838406733</v>
+      </c>
+      <c r="L68" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-3.6543262032828983E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>330</v>
       </c>
@@ -4470,8 +5405,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>4.4150943396226411E-2</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H69">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>5.7595865315812871</v>
+      </c>
+      <c r="I69">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J69">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-26817.607910984363</v>
+      </c>
+      <c r="K69">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>867.35099968455677</v>
+      </c>
+      <c r="L69" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-3.234259381237705E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>340</v>
       </c>
@@ -4493,8 +5448,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>8.2424242424242428E-2</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H70">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>5.9341194567807207</v>
+      </c>
+      <c r="I70">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J70">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-28409.157341903319</v>
+      </c>
+      <c r="K70">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>874.34205543255109</v>
+      </c>
+      <c r="L70" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-3.0776768381753524E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>350</v>
       </c>
@@ -4516,8 +5491,28 @@
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>0.23461538461538461</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H71">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>6.1086523819801526</v>
+      </c>
+      <c r="I71">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J71">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-30000.706772822268</v>
+      </c>
+      <c r="K71">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>881.21046521750645</v>
+      </c>
+      <c r="L71" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-2.9372990172878116E-2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>360</v>
       </c>
@@ -4538,16 +5533,37 @@
       <c r="F72" s="4">
         <f>טבלה1[[#This Row],[dfield]]/טבלה1[[#This Row],[field]]</f>
         <v>0.38643067846607676</v>
+      </c>
+      <c r="H72">
+        <f>טבלה1[[#This Row],[theta(rad)]]</f>
+        <v>6.2831853071795862</v>
+      </c>
+      <c r="I72">
+        <f>טבלה1[[#This Row],[dtheta]]</f>
+        <v>2.886751345948129E-3</v>
+      </c>
+      <c r="J72">
+        <f>(טבלה1[[#This Row],[field]]-B$2)/B$3</f>
+        <v>-30495.678645838067</v>
+      </c>
+      <c r="K72">
+        <f>SQRT(טבלה1[[#This Row],[dfield]]^2 +E$2^2)/B$3</f>
+        <v>872.40611838406733</v>
+      </c>
+      <c r="L72" s="6">
+        <f>טבלה4[[#This Row],[rdfield]]/טבלה4[[#This Row],[rfield]]</f>
+        <v>-2.860753251356582E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
-  <tableParts count="3">
+  <tableParts count="4">
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>